<commit_message>
modifing sql and evaluation sheet
</commit_message>
<xml_diff>
--- a/DB_ Evaluation.xlsx
+++ b/DB_ Evaluation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatma\Desktop\TRA-Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1817C94A-0A8C-4ACA-80AD-331E296B0B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A9A6E0-2BA3-41A1-8AAD-117A885BAE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB Test Result" sheetId="4" r:id="rId1"/>
+    <sheet name="DB Part 1 Project " sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -152,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -161,13 +162,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +511,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -526,19 +526,19 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
@@ -546,17 +546,17 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
@@ -564,17 +564,17 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
@@ -650,27 +650,22 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
-      <c r="N13" s="8"/>
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
-      <c r="N14" s="8"/>
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
-      <c r="N15" s="8"/>
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
-      <c r="N16" s="8"/>
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
-      <c r="N17" s="8"/>
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
@@ -761,4 +756,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958FE5C1-8A4D-489C-BC7D-FDC992B3AFB8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modifing the evaluation sheet
</commit_message>
<xml_diff>
--- a/DB_ Evaluation.xlsx
+++ b/DB_ Evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatma\Desktop\TRA-Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatma\Desktop\all\TRA-Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A9A6E0-2BA3-41A1-8AAD-117A885BAE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E492004B-272D-4F4C-957A-A2DBF8009423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB Test Result" sheetId="4" r:id="rId1"/>
@@ -511,8 +511,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,7 +597,9 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>26</v>
+      </c>
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
@@ -605,7 +607,9 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>26</v>
+      </c>
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -613,7 +617,9 @@
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>41</v>
+      </c>
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -621,7 +627,9 @@
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>43</v>
+      </c>
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -629,7 +637,9 @@
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>38</v>
+      </c>
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
@@ -637,7 +647,9 @@
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>39</v>
+      </c>
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
@@ -645,7 +657,9 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1">
+        <v>34</v>
+      </c>
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
@@ -762,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958FE5C1-8A4D-489C-BC7D-FDC992B3AFB8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>

</xml_diff>